<commit_message>
removed ALP from proposed site list
</commit_message>
<xml_diff>
--- a/data/derived_data/iptds_site_recommendations_20240411.xlsx
+++ b/data/derived_data/iptds_site_recommendations_20240411.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\iptds_data_stash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02144FE-183F-4749-BA19-6FD0F921FA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82934F45-1062-4172-AB4F-8A8EB716166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,9 +432,6 @@
     <t>Upgrade to IS1001 MC to increase read range.</t>
   </si>
   <si>
-    <t>Proposed site not necessary if weir is operated annually and is reliable.</t>
-  </si>
-  <si>
     <t>If transfer to IPTDS O&amp;M project is not desired, ensure long-term funding.</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>If feasible, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA populations from SEMEA.</t>
+  </si>
+  <si>
+    <t>Likely not necessary; a weir is operated near the lower 1 rkm of Alpowa Creek and has generated census estimates in nearly all of the previous 19 years.</t>
   </si>
 </sst>
 </file>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -880,7 +880,7 @@
         <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -900,7 +900,7 @@
         <v>122</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,7 +957,7 @@
         <v>118</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -995,7 +995,7 @@
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
         <v>121</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1136,7 +1136,7 @@
         <v>118</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1156,7 +1156,7 @@
         <v>122</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1276,7 +1276,7 @@
         <v>122</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1347,7 +1347,7 @@
         <v>122</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>121</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
         <v>121</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1494,7 +1494,7 @@
         <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
         <v>121</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1554,7 +1554,7 @@
         <v>121</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1574,7 +1574,7 @@
         <v>121</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>118</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>118</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1762,7 +1762,7 @@
         <v>121</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1816,7 +1816,7 @@
         <v>121</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving forward draft report
</commit_message>
<xml_diff>
--- a/data/derived_data/iptds_site_recommendations_20240411.xlsx
+++ b/data/derived_data/iptds_site_recommendations_20240411.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82934F45-1062-4172-AB4F-8A8EB716166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9986E97D-ECFD-4D44-BD68-539D29D27C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="143">
   <si>
     <t>site_code</t>
   </si>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1194,7 +1194,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C21" s="3">
         <v>45.175659000000003</v>
@@ -1202,7 +1202,9 @@
       <c r="D21" s="3">
         <v>-115.579712</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">

</xml_diff>